<commit_message>
TRICC ped compatible with .py files only
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -67,7 +67,10 @@
     <t xml:space="preserve">label_patient_details</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h2 style="text-align:center;margin-bottom:0px;"&gt;${gender_name}&lt;/h2&gt; &lt;p style="text-align:center;"&gt;Weight: ${p_weight} kg&lt;/p&gt;</t>
+    <t xml:space="preserve">&lt;h2 style="text-align:center;"&gt;${gender_name}&lt;/h2&gt; &lt;p style="text-align:center;"&gt;Weight: ${p_weight} kg&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">center</t>
   </si>
   <si>
     <t xml:space="preserve">calculate</t>
@@ -79,6 +82,9 @@
     <t xml:space="preserve">jr:choice-name(${gender}, '${gender}')</t>
   </si>
   <si>
+    <t xml:space="preserve">g_diagnosis</t>
+  </si>
+  <si>
     <t xml:space="preserve">label_summary</t>
   </si>
   <si>
@@ -89,6 +95,21 @@
   </si>
   <si>
     <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g_danger_signs_summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observed danger signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_danger_signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danger signs&lt;i class="fa fa-user"&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 red</t>
   </si>
 </sst>
 </file>
@@ -526,15 +547,15 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="6" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="8.36"/>
@@ -602,51 +623,59 @@
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -654,44 +683,92 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="E1 B1:D8">
+  <conditionalFormatting sqref="E1 B1:D12">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1 B1:C8">
+  <conditionalFormatting sqref="E1 B1:C12">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D8">
+  <conditionalFormatting sqref="B1:D12">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D8 B1:C8">
+  <conditionalFormatting sqref="D11:D12 B1:C12">
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7:D8 B1:C8">
+  <conditionalFormatting sqref="D11:D12 B1:C12">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D8">
+  <conditionalFormatting sqref="B1:D12">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C8">
+  <conditionalFormatting sqref="B1:C12">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>$A1="note"</formula>
     </cfRule>
@@ -702,17 +779,17 @@
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1 B1:B8">
+  <conditionalFormatting sqref="F1 B1:B12">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D8">
+  <conditionalFormatting sqref="B1:D12">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D8 A1:C8 D1:F1">
+  <conditionalFormatting sqref="D2:D12 A1:C12 D1:F1">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
@@ -756,13 +833,13 @@
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B8">
+  <conditionalFormatting sqref="B1:B12">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>